<commit_message>
save "Indonesia" in v2
</commit_message>
<xml_diff>
--- a/Data/country_data/country_risk_premium.xlsx
+++ b/Data/country_data/country_risk_premium.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canne\Documents\MFE Winter\230O\prem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A001179-A0D6-48AE-8A86-44512808EBA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2532" yWindow="1176" windowWidth="20508" windowHeight="11184" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Argentina</t>
   </si>
@@ -38,9 +44,6 @@
   </si>
   <si>
     <t>India</t>
-  </si>
-  <si>
-    <t>Indonesia</t>
   </si>
   <si>
     <t>Korea</t>
@@ -91,8 +94,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +158,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -201,7 +212,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,9 +244,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,6 +296,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,14 +489,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>2000</v>
       </c>
@@ -514,42 +563,42 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.055</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C2">
         <v>0.09</v>
       </c>
       <c r="D2">
-        <v>0.135</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="E2">
-        <v>0.0975</v>
+        <v>9.7500000000000003E-2</v>
       </c>
       <c r="F2">
-        <v>0.0975</v>
+        <v>9.7500000000000003E-2</v>
       </c>
       <c r="G2">
-        <v>0.09000000000000001</v>
+        <v>9.0000000000000011E-2</v>
       </c>
       <c r="H2">
-        <v>0.0675</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="I2">
-        <v>0.0675</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="J2">
-        <v>0.135</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="K2">
-        <v>0.09750000000000002</v>
+        <v>9.7500000000000017E-2</v>
       </c>
       <c r="L2">
-        <v>0.09000000000000001</v>
+        <v>9.0000000000000011E-2</v>
       </c>
       <c r="M2">
         <v>0.09</v>
@@ -558,7 +607,7 @@
         <v>0.09</v>
       </c>
       <c r="O2">
-        <v>0.0975</v>
+        <v>9.7500000000000003E-2</v>
       </c>
       <c r="P2">
         <v>0.1125</v>
@@ -567,51 +616,51 @@
         <v>0.10206</v>
       </c>
       <c r="R2">
-        <v>0.09246009595142002</v>
+        <v>9.2460095951420018E-2</v>
       </c>
       <c r="S2">
-        <v>0.06344164373946019</v>
+        <v>6.3441643739460193E-2</v>
       </c>
       <c r="T2">
-        <v>0.07638151563795058</v>
+        <v>7.6381515637950578E-2</v>
       </c>
       <c r="U2">
-        <v>0.08879630867759671</v>
+        <v>8.8796308677596705E-2</v>
       </c>
       <c r="V2">
         <v>0.1162057965865632</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.04499999999999999</v>
+        <v>4.4999999999999991E-2</v>
       </c>
       <c r="C3">
-        <v>0.04499999999999999</v>
+        <v>4.4999999999999991E-2</v>
       </c>
       <c r="D3">
         <v>0.1125</v>
       </c>
       <c r="E3">
-        <v>0.08250000000000002</v>
+        <v>8.2500000000000018E-2</v>
       </c>
       <c r="F3">
         <v>0.06</v>
       </c>
       <c r="G3">
-        <v>0.05399999999999999</v>
+        <v>5.3999999999999992E-2</v>
       </c>
       <c r="H3">
-        <v>0.03750000000000001</v>
+        <v>3.7500000000000012E-2</v>
       </c>
       <c r="I3">
         <v>0.03</v>
       </c>
       <c r="J3">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="K3">
         <v>0.03</v>
@@ -620,202 +669,202 @@
         <v>0.03</v>
       </c>
       <c r="M3">
-        <v>0.02625</v>
+        <v>2.6249999999999999E-2</v>
       </c>
       <c r="N3">
-        <v>0.02625</v>
+        <v>2.6249999999999999E-2</v>
       </c>
       <c r="O3">
-        <v>0.0285</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="P3">
-        <v>0.0285</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="Q3">
-        <v>0.04718</v>
+        <v>4.718E-2</v>
       </c>
       <c r="R3">
-        <v>0.04270348398311077</v>
+        <v>4.2703483983110767E-2</v>
       </c>
       <c r="S3">
-        <v>0.03463289732006598</v>
+        <v>3.4632897320065983E-2</v>
       </c>
       <c r="T3">
-        <v>0.04169679460235663</v>
+        <v>4.1696794602356632E-2</v>
       </c>
       <c r="U3">
-        <v>0.02962842764492955</v>
+        <v>2.962842764492955E-2</v>
       </c>
       <c r="V3">
-        <v>0.02909513553633499</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
+        <v>2.9095135536334991E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="C4">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D4">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E4">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F4">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="G4">
-        <v>0.009000000000000001</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="H4">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="I4">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="J4">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="K4">
-        <v>0.0135</v>
+        <v>1.35E-2</v>
       </c>
       <c r="L4">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="M4">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="N4">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="O4">
-        <v>0.009000000000000001</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="P4">
-        <v>0.009000000000000001</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="Q4">
-        <v>0.009519999999999999</v>
+        <v>9.5199999999999989E-3</v>
       </c>
       <c r="R4">
-        <v>0.008591992272878143</v>
+        <v>8.5919922728781434E-3</v>
       </c>
       <c r="S4">
-        <v>0.006968180541875137</v>
+        <v>6.9681805418751368E-3</v>
       </c>
       <c r="T4">
-        <v>0.009766816753705157</v>
+        <v>9.7668167537051567E-3</v>
       </c>
       <c r="U4">
-        <v>0.006939992060974491</v>
+        <v>6.9399920609744909E-3</v>
       </c>
       <c r="V4">
-        <v>0.006815076792294684</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
+        <v>6.8150767922946836E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.009500000000000001</v>
+        <v>9.5000000000000015E-3</v>
       </c>
       <c r="C5">
-        <v>0.009500000000000001</v>
+        <v>9.5000000000000015E-3</v>
       </c>
       <c r="D5">
-        <v>0.02025</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="E5">
-        <v>0.0135</v>
+        <v>1.35E-2</v>
       </c>
       <c r="F5">
-        <v>0.0135</v>
+        <v>1.35E-2</v>
       </c>
       <c r="G5">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H5">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I5">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="J5">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="K5">
-        <v>0.0135</v>
+        <v>1.35E-2</v>
       </c>
       <c r="L5">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="M5">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="N5">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="O5">
-        <v>0.009000000000000001</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="P5">
-        <v>0.009000000000000001</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="Q5">
-        <v>0.009519999999999999</v>
+        <v>9.5199999999999989E-3</v>
       </c>
       <c r="R5">
-        <v>0.008591992272878143</v>
+        <v>8.5919922728781434E-3</v>
       </c>
       <c r="S5">
-        <v>0.008112210183078518</v>
+        <v>8.1122101830785175E-3</v>
       </c>
       <c r="T5">
-        <v>0.009766816753705157</v>
+        <v>9.7668167537051567E-3</v>
       </c>
       <c r="U5">
-        <v>0.006939992060974491</v>
+        <v>6.9399920609744909E-3</v>
       </c>
       <c r="V5">
-        <v>0.006815076792294684</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
+        <v>6.8150767922946836E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.03000000000000001</v>
+        <v>3.0000000000000009E-2</v>
       </c>
       <c r="C6">
-        <v>0.03000000000000001</v>
+        <v>3.0000000000000009E-2</v>
       </c>
       <c r="D6">
-        <v>0.02625</v>
+        <v>2.6249999999999999E-2</v>
       </c>
       <c r="E6">
-        <v>0.0195</v>
+        <v>1.95E-2</v>
       </c>
       <c r="F6">
-        <v>0.0195</v>
+        <v>1.95E-2</v>
       </c>
       <c r="G6">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="H6">
-        <v>0.02025</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="I6">
-        <v>0.02025</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="J6">
-        <v>0.03899999999999999</v>
+        <v>3.8999999999999993E-2</v>
       </c>
       <c r="K6">
         <v>0.03</v>
@@ -830,72 +879,72 @@
         <v>0.03</v>
       </c>
       <c r="O6">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="P6">
-        <v>0.0285</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="Q6">
-        <v>0.02982</v>
+        <v>2.9819999999999999E-2</v>
       </c>
       <c r="R6">
-        <v>0.02705836372503415</v>
+        <v>2.7058363725034149E-2</v>
       </c>
       <c r="S6">
-        <v>0.02194456857217394</v>
+        <v>2.1944568572173941E-2</v>
       </c>
       <c r="T6">
-        <v>0.02642049147476651</v>
+        <v>2.6420491474766512E-2</v>
       </c>
       <c r="U6">
-        <v>0.01877356826750792</v>
+        <v>1.8773568267507919E-2</v>
       </c>
       <c r="V6">
-        <v>0.018435656450951</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
+        <v>1.8435656450951E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C7">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D7">
-        <v>0.02249999999999999</v>
+        <v>2.2499999999999989E-2</v>
       </c>
       <c r="E7">
-        <v>0.01800000000000001</v>
+        <v>1.8000000000000009E-2</v>
       </c>
       <c r="F7">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G7">
-        <v>0.02025</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="H7">
-        <v>0.02025</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="I7">
-        <v>0.02025</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="J7">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="K7">
-        <v>0.03750000000000001</v>
+        <v>3.7500000000000012E-2</v>
       </c>
       <c r="L7">
-        <v>0.036</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="M7">
-        <v>0.07500000000000001</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="N7">
-        <v>0.07500000000000001</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="O7">
         <v>0.1125</v>
@@ -907,57 +956,57 @@
         <v>0.10206</v>
       </c>
       <c r="R7">
-        <v>0.09246009595142002</v>
+        <v>9.2460095951420018E-2</v>
       </c>
       <c r="S7">
-        <v>0.07498594284614887</v>
+        <v>7.4985942846148873E-2</v>
       </c>
       <c r="T7">
-        <v>0.09028044717206947</v>
+        <v>9.028044717206947E-2</v>
       </c>
       <c r="U7">
-        <v>0.05427429688710819</v>
+        <v>5.4274296887108192E-2</v>
       </c>
       <c r="V7">
-        <v>0.05329739542691996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
+        <v>5.3297395426919962E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.009500000000000001</v>
+        <v>9.5000000000000015E-3</v>
       </c>
       <c r="C8">
-        <v>0.005999999999999998</v>
+        <v>5.9999999999999984E-3</v>
       </c>
       <c r="D8">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E8">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F8">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="G8">
-        <v>0.009000000000000001</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="H8">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="I8">
-        <v>0.0105</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="J8">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="K8">
-        <v>0.01575</v>
+        <v>1.575E-2</v>
       </c>
       <c r="L8">
-        <v>0.036</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="M8">
         <v>0.105</v>
@@ -981,51 +1030,51 @@
         <v>0.1037946892655431</v>
       </c>
       <c r="T8">
-        <v>0.09028044717206947</v>
+        <v>9.028044717206947E-2</v>
       </c>
       <c r="U8">
-        <v>0.04439815433879835</v>
+        <v>4.4398154338798353E-2</v>
       </c>
       <c r="V8">
-        <v>0.03486173897596896</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
+        <v>3.4861738975968962E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.03000000000000001</v>
+        <v>3.0000000000000009E-2</v>
       </c>
       <c r="C9">
-        <v>0.03000000000000001</v>
+        <v>3.0000000000000009E-2</v>
       </c>
       <c r="D9">
         <v>0.06</v>
       </c>
       <c r="E9">
-        <v>0.02175</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F9">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G9">
-        <v>0.04049999999999999</v>
+        <v>4.0499999999999987E-2</v>
       </c>
       <c r="H9">
-        <v>0.03750000000000001</v>
+        <v>3.7500000000000012E-2</v>
       </c>
       <c r="I9">
-        <v>0.03750000000000001</v>
+        <v>3.7500000000000012E-2</v>
       </c>
       <c r="J9">
         <v>0.06</v>
       </c>
       <c r="K9">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="L9">
-        <v>0.036</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="M9">
         <v>0.03</v>
@@ -1034,1116 +1083,1048 @@
         <v>0.03</v>
       </c>
       <c r="O9">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="P9">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="Q9">
-        <v>0.03458</v>
+        <v>3.458E-2</v>
       </c>
       <c r="R9">
-        <v>0.03129024051615324</v>
+        <v>3.1290240516153242E-2</v>
       </c>
       <c r="S9">
-        <v>0.02194456857217394</v>
+        <v>2.1944568572173941E-2</v>
       </c>
       <c r="T9">
-        <v>0.02642049147476651</v>
+        <v>2.6420491474766512E-2</v>
       </c>
       <c r="U9">
-        <v>0.01877356826750792</v>
+        <v>1.8773568267507919E-2</v>
       </c>
       <c r="V9">
-        <v>0.02131895817076799</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
+        <v>2.1318958170767989E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.065</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="C10">
-        <v>0.065</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D10">
-        <v>0.1275</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="E10">
-        <v>0.08250000000000002</v>
+        <v>1.4250000000000001E-2</v>
       </c>
       <c r="F10">
-        <v>0.08250000000000002</v>
+        <v>1.4250000000000001E-2</v>
       </c>
       <c r="G10">
-        <v>0.07500000000000001</v>
+        <v>1.35E-2</v>
       </c>
       <c r="H10">
-        <v>0.0525</v>
+        <v>1.2749999999999999E-2</v>
       </c>
       <c r="I10">
-        <v>0.045</v>
+        <v>1.2E-2</v>
       </c>
       <c r="J10">
-        <v>0.07875</v>
+        <v>2.4000000000000011E-2</v>
       </c>
       <c r="K10">
-        <v>0.045</v>
+        <v>1.575E-2</v>
       </c>
       <c r="L10">
-        <v>0.04125</v>
+        <v>1.2749999999999999E-2</v>
       </c>
       <c r="M10">
-        <v>0.036</v>
+        <v>1.2749999999999999E-2</v>
       </c>
       <c r="N10">
-        <v>0.03</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="O10">
-        <v>0.033</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="P10">
-        <v>0.033</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="Q10">
-        <v>0.03458</v>
+        <v>7.8399999999999997E-3</v>
       </c>
       <c r="R10">
-        <v>0.03129024051615324</v>
+        <v>7.0531279851984751E-3</v>
       </c>
       <c r="S10">
-        <v>0.02537665749578408</v>
+        <v>5.7201482060169036E-3</v>
       </c>
       <c r="T10">
-        <v>0.02642049147476651</v>
+        <v>6.8868579673562009E-3</v>
       </c>
       <c r="U10">
-        <v>0.01877356826750792</v>
+        <v>4.8935841455589359E-3</v>
       </c>
       <c r="V10">
-        <v>0.018435656450951</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
+        <v>4.8055028663616358E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.013</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="C11">
-        <v>0.013</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D11">
-        <v>0.02025</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="E11">
-        <v>0.01425</v>
+        <v>1.4250000000000001E-2</v>
       </c>
       <c r="F11">
-        <v>0.01425</v>
+        <v>1.4250000000000001E-2</v>
       </c>
       <c r="G11">
-        <v>0.0135</v>
+        <v>1.35E-2</v>
       </c>
       <c r="H11">
-        <v>0.01275</v>
+        <v>1.2749999999999999E-2</v>
       </c>
       <c r="I11">
-        <v>0.012</v>
+        <v>1.2749999999999999E-2</v>
       </c>
       <c r="J11">
-        <v>0.02400000000000001</v>
+        <v>2.6250000000000009E-2</v>
       </c>
       <c r="K11">
-        <v>0.01575</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="L11">
-        <v>0.01275</v>
+        <v>1.7250000000000001E-2</v>
       </c>
       <c r="M11">
-        <v>0.01275</v>
+        <v>1.7250000000000001E-2</v>
       </c>
       <c r="N11">
-        <v>0.0105</v>
+        <v>1.7250000000000001E-2</v>
       </c>
       <c r="O11">
-        <v>0.009000000000000001</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="P11">
-        <v>0.009000000000000001</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="Q11">
-        <v>0.00784</v>
+        <v>1.89E-2</v>
       </c>
       <c r="R11">
-        <v>0.007053127985198475</v>
+        <v>1.7055745855116319E-2</v>
       </c>
       <c r="S11">
-        <v>0.005720148206016904</v>
+        <v>1.383235838909542E-2</v>
       </c>
       <c r="T11">
-        <v>0.006886857967356201</v>
+        <v>1.665367472106136E-2</v>
       </c>
       <c r="U11">
-        <v>0.004893584145558936</v>
+        <v>1.1833576206533429E-2</v>
       </c>
       <c r="V11">
-        <v>0.004805502866361636</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
+        <v>1.1620579658656319E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.013</v>
+        <v>1.4500000000000009E-2</v>
       </c>
       <c r="C12">
-        <v>0.013</v>
+        <v>1.4500000000000009E-2</v>
       </c>
       <c r="D12">
-        <v>0.02025</v>
+        <v>2.2499999999999989E-2</v>
       </c>
       <c r="E12">
-        <v>0.01425</v>
+        <v>1.8000000000000009E-2</v>
       </c>
       <c r="F12">
-        <v>0.01425</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G12">
-        <v>0.0135</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="H12">
-        <v>0.01275</v>
+        <v>1.4999999999999991E-2</v>
       </c>
       <c r="I12">
-        <v>0.01275</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="J12">
-        <v>0.02625000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="K12">
-        <v>0.018</v>
+        <v>2.4000000000000011E-2</v>
       </c>
       <c r="L12">
-        <v>0.01725</v>
+        <v>2.250000000000001E-2</v>
       </c>
       <c r="M12">
-        <v>0.01725</v>
+        <v>2.2499999999999989E-2</v>
       </c>
       <c r="N12">
-        <v>0.01725</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="O12">
-        <v>0.018</v>
+        <v>2.4E-2</v>
       </c>
       <c r="P12">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="Q12">
-        <v>0.0189</v>
+        <v>1.89E-2</v>
       </c>
       <c r="R12">
-        <v>0.01705574585511632</v>
+        <v>1.7055745855116319E-2</v>
       </c>
       <c r="S12">
-        <v>0.01383235838909542</v>
+        <v>1.383235838909542E-2</v>
       </c>
       <c r="T12">
-        <v>0.01665367472106136</v>
+        <v>1.665367472106136E-2</v>
       </c>
       <c r="U12">
-        <v>0.01183357620653343</v>
+        <v>1.1833576206533429E-2</v>
       </c>
       <c r="V12">
-        <v>0.01162057965865632</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
+        <v>1.5464981951745629E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.01450000000000001</v>
+        <v>7.4999999999999983E-2</v>
       </c>
       <c r="C13">
-        <v>0.01450000000000001</v>
+        <v>7.4999999999999983E-2</v>
       </c>
       <c r="D13">
-        <v>0.02249999999999999</v>
+        <v>0.1275</v>
       </c>
       <c r="E13">
-        <v>0.01800000000000001</v>
+        <v>8.2500000000000018E-2</v>
       </c>
       <c r="F13">
-        <v>0.018</v>
+        <v>8.2500000000000018E-2</v>
       </c>
       <c r="G13">
-        <v>0.0165</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="H13">
-        <v>0.01499999999999999</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="I13">
-        <v>0.015</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="J13">
-        <v>0.03</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="K13">
-        <v>0.02400000000000001</v>
+        <v>9.7500000000000017E-2</v>
       </c>
       <c r="L13">
-        <v>0.02250000000000001</v>
+        <v>9.0000000000000011E-2</v>
       </c>
       <c r="M13">
-        <v>0.02249999999999999</v>
+        <v>0.09</v>
       </c>
       <c r="N13">
-        <v>0.0225</v>
+        <v>0.105</v>
       </c>
       <c r="O13">
-        <v>0.024</v>
+        <v>0.1125</v>
       </c>
       <c r="P13">
-        <v>0.018</v>
+        <v>0.1125</v>
       </c>
       <c r="Q13">
-        <v>0.0189</v>
+        <v>0.10206</v>
       </c>
       <c r="R13">
-        <v>0.01705574585511632</v>
+        <v>9.2460095951420018E-2</v>
       </c>
       <c r="S13">
-        <v>0.01383235838909542</v>
+        <v>7.4985942846148873E-2</v>
       </c>
       <c r="T13">
-        <v>0.01665367472106136</v>
+        <v>9.028044717206947E-2</v>
       </c>
       <c r="U13">
-        <v>0.01183357620653343</v>
+        <v>6.4150439435418039E-2</v>
       </c>
       <c r="V13">
-        <v>0.01546498195174563</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
+        <v>6.2995773939031607E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.07499999999999998</v>
+        <v>0.04</v>
       </c>
       <c r="C14">
-        <v>0.07499999999999998</v>
+        <v>0.04</v>
       </c>
       <c r="D14">
-        <v>0.1275</v>
+        <v>0.03</v>
       </c>
       <c r="E14">
-        <v>0.08250000000000002</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F14">
-        <v>0.08250000000000002</v>
+        <v>2.1750000000000009E-2</v>
       </c>
       <c r="G14">
-        <v>0.07500000000000001</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="H14">
-        <v>0.0525</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="I14">
-        <v>0.0525</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="J14">
-        <v>0.135</v>
+        <v>3.8999999999999993E-2</v>
       </c>
       <c r="K14">
-        <v>0.09750000000000002</v>
+        <v>0.03</v>
       </c>
       <c r="L14">
-        <v>0.09000000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="M14">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
       <c r="N14">
-        <v>0.105</v>
+        <v>2.6249999999999999E-2</v>
       </c>
       <c r="O14">
-        <v>0.1125</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="P14">
-        <v>0.1125</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="Q14">
-        <v>0.10206</v>
+        <v>1.89E-2</v>
       </c>
       <c r="R14">
-        <v>0.09246009595142002</v>
+        <v>1.7055745855116319E-2</v>
       </c>
       <c r="S14">
-        <v>0.07498594284614887</v>
+        <v>1.383235838909542E-2</v>
       </c>
       <c r="T14">
-        <v>0.09028044717206947</v>
+        <v>1.665367472106136E-2</v>
       </c>
       <c r="U14">
-        <v>0.06415043943541804</v>
+        <v>1.1833576206533429E-2</v>
       </c>
       <c r="V14">
-        <v>0.06299577393903161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
+        <v>1.1620579658656319E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.04</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C15">
-        <v>0.04</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D15">
         <v>0.03</v>
       </c>
       <c r="E15">
-        <v>0.02175</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F15">
-        <v>0.02175000000000001</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G15">
-        <v>0.02025</v>
+        <v>0.06</v>
       </c>
       <c r="H15">
-        <v>0.02025</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="I15">
-        <v>0.02025</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="J15">
-        <v>0.03899999999999999</v>
+        <v>9.7500000000000017E-2</v>
       </c>
       <c r="K15">
-        <v>0.03</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="L15">
-        <v>0.03</v>
+        <v>4.8750000000000002E-2</v>
       </c>
       <c r="M15">
-        <v>0.03</v>
+        <v>4.1250000000000009E-2</v>
       </c>
       <c r="N15">
-        <v>0.02625</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="O15">
-        <v>0.0285</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="P15">
-        <v>0.018</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="Q15">
-        <v>0.0189</v>
+        <v>2.9819999999999999E-2</v>
       </c>
       <c r="R15">
-        <v>0.01705574585511632</v>
+        <v>2.7058363725034149E-2</v>
       </c>
       <c r="S15">
-        <v>0.01383235838909542</v>
+        <v>2.1944568572173941E-2</v>
       </c>
       <c r="T15">
-        <v>0.01665367472106136</v>
+        <v>2.6420491474766512E-2</v>
       </c>
       <c r="U15">
-        <v>0.01183357620653343</v>
+        <v>1.8773568267507919E-2</v>
       </c>
       <c r="V15">
-        <v>0.01162057965865632</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
+        <v>1.8435656450951E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.025</v>
+        <v>1.2E-2</v>
       </c>
       <c r="C16">
-        <v>0.025</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D16">
-        <v>0.03</v>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="E16">
-        <v>0.02175</v>
+        <v>1.35E-2</v>
       </c>
       <c r="F16">
-        <v>0.045</v>
+        <v>1.35E-2</v>
       </c>
       <c r="G16">
-        <v>0.06</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H16">
-        <v>0.0525</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I16">
-        <v>0.0525</v>
+        <v>1.2E-2</v>
       </c>
       <c r="J16">
-        <v>0.09750000000000002</v>
+        <v>2.4000000000000011E-2</v>
       </c>
       <c r="K16">
-        <v>0.0525</v>
+        <v>1.575E-2</v>
       </c>
       <c r="L16">
-        <v>0.04875</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="M16">
-        <v>0.04125000000000001</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="N16">
-        <v>0.036</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="O16">
-        <v>0.033</v>
+        <v>1.2749999999999999E-2</v>
       </c>
       <c r="P16">
-        <v>0.0285</v>
+        <v>1.2749999999999999E-2</v>
       </c>
       <c r="Q16">
-        <v>0.02982</v>
+        <v>1.3299999999999999E-2</v>
       </c>
       <c r="R16">
-        <v>0.02705836372503415</v>
+        <v>1.20544369201574E-2</v>
       </c>
       <c r="S16">
-        <v>0.02194456857217394</v>
+        <v>9.7762532975561641E-3</v>
       </c>
       <c r="T16">
-        <v>0.02642049147476651</v>
+        <v>1.1770266344208779E-2</v>
       </c>
       <c r="U16">
-        <v>0.01877356826750792</v>
+        <v>8.36358017604618E-3</v>
       </c>
       <c r="V16">
-        <v>0.018435656450951</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
+        <v>8.2130412625089771E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.012</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="C17">
-        <v>0.012</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D17">
-        <v>0.01875</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="E17">
-        <v>0.0135</v>
+        <v>1.4250000000000001E-2</v>
       </c>
       <c r="F17">
-        <v>0.0135</v>
+        <v>1.4250000000000001E-2</v>
       </c>
       <c r="G17">
-        <v>0.012</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="H17">
-        <v>0.012</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="I17">
-        <v>0.012</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="J17">
-        <v>0.02400000000000001</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K17">
-        <v>0.01575</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="L17">
-        <v>0.015</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="M17">
-        <v>0.015</v>
+        <v>7.5000000000000067E-3</v>
       </c>
       <c r="N17">
-        <v>0.015</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="O17">
-        <v>0.01275</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="P17">
-        <v>0.01275</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="Q17">
-        <v>0.0133</v>
+        <v>7.8399999999999997E-3</v>
       </c>
       <c r="R17">
-        <v>0.0120544369201574</v>
+        <v>7.0531279851984751E-3</v>
       </c>
       <c r="S17">
-        <v>0.009776253297556164</v>
+        <v>6.9681805418751368E-3</v>
       </c>
       <c r="T17">
-        <v>0.01177026634420878</v>
+        <v>8.389445160233917E-3</v>
       </c>
       <c r="U17">
-        <v>0.00836358017604618</v>
+        <v>5.9612752318627038E-3</v>
       </c>
       <c r="V17">
-        <v>0.008213041262508977</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22">
+        <v>5.8539762190223561E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.013</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C18">
-        <v>0.013</v>
+        <v>0.04</v>
       </c>
       <c r="D18">
-        <v>0.02025</v>
+        <v>0.06</v>
       </c>
       <c r="E18">
-        <v>0.01425</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="F18">
-        <v>0.01425</v>
+        <v>2.1750000000000009E-2</v>
       </c>
       <c r="G18">
-        <v>0.009000000000000001</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="H18">
-        <v>0.009000000000000001</v>
+        <v>1.7249999999999991E-2</v>
       </c>
       <c r="I18">
-        <v>0.0075</v>
+        <v>1.7250000000000001E-2</v>
       </c>
       <c r="J18">
-        <v>0.015</v>
+        <v>0.03</v>
       </c>
       <c r="K18">
-        <v>0.009000000000000001</v>
+        <v>2.4000000000000011E-2</v>
       </c>
       <c r="L18">
-        <v>0.0075</v>
+        <v>2.250000000000001E-2</v>
       </c>
       <c r="M18">
-        <v>0.007500000000000007</v>
+        <v>2.2499999999999989E-2</v>
       </c>
       <c r="N18">
-        <v>0.0075</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="O18">
-        <v>0.0075</v>
+        <v>2.4E-2</v>
       </c>
       <c r="P18">
-        <v>0.0075</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="Q18">
-        <v>0.00784</v>
+        <v>3.9199999999999999E-2</v>
       </c>
       <c r="R18">
-        <v>0.007053127985198475</v>
+        <v>3.5522117307272318E-2</v>
       </c>
       <c r="S18">
-        <v>0.006968180541875137</v>
+        <v>2.880874641939422E-2</v>
       </c>
       <c r="T18">
-        <v>0.008389445160233917</v>
+        <v>3.468472103559396E-2</v>
       </c>
       <c r="U18">
-        <v>0.005961275231862704</v>
+        <v>2.1709718754843281E-2</v>
       </c>
       <c r="V18">
-        <v>0.005853976219022356</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
+        <v>2.1318958170767989E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.055</v>
+        <v>1.4500000000000009E-2</v>
       </c>
       <c r="C19">
-        <v>0.04</v>
+        <v>1.4500000000000009E-2</v>
       </c>
       <c r="D19">
-        <v>0.06</v>
+        <v>4.8750000000000002E-2</v>
       </c>
       <c r="E19">
-        <v>0.02175</v>
+        <v>1.8000000000000009E-2</v>
       </c>
       <c r="F19">
-        <v>0.02175000000000001</v>
+        <v>1.95E-2</v>
       </c>
       <c r="G19">
-        <v>0.018</v>
+        <v>1.35E-2</v>
       </c>
       <c r="H19">
-        <v>0.01724999999999999</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I19">
-        <v>0.01725</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="J19">
-        <v>0.03</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="K19">
-        <v>0.02400000000000001</v>
+        <v>1.35E-2</v>
       </c>
       <c r="L19">
-        <v>0.02250000000000001</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="M19">
-        <v>0.02249999999999999</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="N19">
-        <v>0.0225</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="O19">
-        <v>0.024</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="P19">
-        <v>0.0285</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="Q19">
-        <v>0.0392</v>
+        <v>1.106E-2</v>
       </c>
       <c r="R19">
-        <v>0.03552211730727232</v>
+        <v>1.0002617869917839E-2</v>
       </c>
       <c r="S19">
-        <v>0.02880874641939422</v>
+        <v>8.1122101830785175E-3</v>
       </c>
       <c r="T19">
-        <v>0.03468472103559396</v>
+        <v>9.7668167537051567E-3</v>
       </c>
       <c r="U19">
-        <v>0.02170971875484328</v>
+        <v>6.9399920609744909E-3</v>
       </c>
       <c r="V19">
-        <v>0.02131895817076799</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
+        <v>6.8150767922946836E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.01450000000000001</v>
+        <v>1.4500000000000009E-2</v>
       </c>
       <c r="C20">
-        <v>0.01450000000000001</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D20">
-        <v>0.04875</v>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="E20">
-        <v>0.01800000000000001</v>
+        <v>1.35E-2</v>
       </c>
       <c r="F20">
-        <v>0.0195</v>
+        <v>1.35E-2</v>
       </c>
       <c r="G20">
-        <v>0.0135</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H20">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I20">
-        <v>0.0105</v>
+        <v>1.2E-2</v>
       </c>
       <c r="J20">
-        <v>0.021</v>
+        <v>2.4000000000000011E-2</v>
       </c>
       <c r="K20">
-        <v>0.0135</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="L20">
-        <v>0.0105</v>
+        <v>1.7250000000000001E-2</v>
       </c>
       <c r="M20">
-        <v>0.0105</v>
+        <v>1.7250000000000001E-2</v>
       </c>
       <c r="N20">
-        <v>0.0105</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="O20">
-        <v>0.009000000000000001</v>
+        <v>2.4E-2</v>
       </c>
       <c r="P20">
-        <v>0.009000000000000001</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="Q20">
-        <v>0.01106</v>
+        <v>2.9819999999999999E-2</v>
       </c>
       <c r="R20">
-        <v>0.01000261786991784</v>
+        <v>2.7058363725034149E-2</v>
       </c>
       <c r="S20">
-        <v>0.008112210183078518</v>
+        <v>2.5376657495784081E-2</v>
       </c>
       <c r="T20">
-        <v>0.009766816753705157</v>
+        <v>3.0552606255180231E-2</v>
       </c>
       <c r="U20">
-        <v>0.006939992060974491</v>
+        <v>2.1709718754843281E-2</v>
       </c>
       <c r="V20">
-        <v>0.006815076792294684</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22">
+        <v>2.9095135536334991E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.01450000000000001</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="C21">
-        <v>0.013</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="D21">
-        <v>0.01875</v>
+        <v>1.35E-2</v>
       </c>
       <c r="E21">
-        <v>0.0135</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="F21">
-        <v>0.0135</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="G21">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>0.012</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="I21">
-        <v>0.012</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="J21">
-        <v>0.02400000000000001</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="K21">
-        <v>0.018</v>
+        <v>1.125E-2</v>
       </c>
       <c r="L21">
-        <v>0.01725</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="M21">
-        <v>0.01725</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="N21">
-        <v>0.0225</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="O21">
-        <v>0.024</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="P21">
-        <v>0.0285</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="Q21">
-        <v>0.02982</v>
+        <v>9.5199999999999989E-3</v>
       </c>
       <c r="R21">
-        <v>0.02705836372503415</v>
+        <v>8.5919922728781434E-3</v>
       </c>
       <c r="S21">
-        <v>0.02537665749578408</v>
+        <v>6.9681805418751368E-3</v>
       </c>
       <c r="T21">
-        <v>0.03055260625518023</v>
+        <v>8.389445160233917E-3</v>
       </c>
       <c r="U21">
-        <v>0.02170971875484328</v>
+        <v>5.9612752318627038E-3</v>
       </c>
       <c r="V21">
-        <v>0.02909513553633499</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22">
+        <v>5.8539762190223561E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.006999999999999999</v>
+        <v>1.4500000000000009E-2</v>
       </c>
       <c r="C22">
-        <v>0.006999999999999999</v>
+        <v>1.4500000000000009E-2</v>
       </c>
       <c r="D22">
-        <v>0.0135</v>
+        <v>2.2499999999999989E-2</v>
       </c>
       <c r="E22">
-        <v>0.0105</v>
+        <v>1.8000000000000009E-2</v>
       </c>
       <c r="F22">
-        <v>0.0105</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="H22">
-        <v>0.009000000000000001</v>
+        <v>1.4999999999999991E-2</v>
       </c>
       <c r="I22">
-        <v>0.009000000000000001</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="J22">
-        <v>0.018</v>
+        <v>0.03</v>
       </c>
       <c r="K22">
-        <v>0.01125</v>
+        <v>2.4000000000000011E-2</v>
       </c>
       <c r="L22">
-        <v>0.0105</v>
+        <v>2.250000000000001E-2</v>
       </c>
       <c r="M22">
-        <v>0.0105</v>
+        <v>2.2499999999999989E-2</v>
       </c>
       <c r="N22">
-        <v>0.0105</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="O22">
-        <v>0.009000000000000001</v>
+        <v>2.4E-2</v>
       </c>
       <c r="P22">
-        <v>0.009000000000000001</v>
+        <v>2.4E-2</v>
       </c>
       <c r="Q22">
-        <v>0.009519999999999999</v>
+        <v>2.5059999999999999E-2</v>
       </c>
       <c r="R22">
-        <v>0.008591992272878143</v>
+        <v>2.2698248243275099E-2</v>
       </c>
       <c r="S22">
-        <v>0.006968180541875137</v>
+        <v>1.8408476953908941E-2</v>
       </c>
       <c r="T22">
-        <v>0.008389445160233917</v>
+        <v>2.2163161094946319E-2</v>
       </c>
       <c r="U22">
-        <v>0.005961275231862704</v>
+        <v>1.574844352298058E-2</v>
       </c>
       <c r="V22">
-        <v>0.005853976219022356</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22">
+        <v>1.5464981951745629E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.01450000000000001</v>
+        <v>4.4999999999999991E-2</v>
       </c>
       <c r="C23">
-        <v>0.01450000000000001</v>
+        <v>4.4999999999999991E-2</v>
       </c>
       <c r="D23">
-        <v>0.02249999999999999</v>
+        <v>0.1275</v>
       </c>
       <c r="E23">
-        <v>0.01800000000000001</v>
+        <v>9.7500000000000003E-2</v>
       </c>
       <c r="F23">
-        <v>0.018</v>
+        <v>8.2500000000000018E-2</v>
       </c>
       <c r="G23">
-        <v>0.0165</v>
+        <v>5.3999999999999992E-2</v>
       </c>
       <c r="H23">
-        <v>0.01499999999999999</v>
+        <v>4.4999999999999991E-2</v>
       </c>
       <c r="I23">
-        <v>0.015</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="J23">
-        <v>0.03</v>
+        <v>7.8750000000000001E-2</v>
       </c>
       <c r="K23">
-        <v>0.02400000000000001</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="L23">
-        <v>0.02250000000000001</v>
+        <v>4.1250000000000002E-2</v>
       </c>
       <c r="M23">
-        <v>0.02249999999999999</v>
+        <v>4.1250000000000009E-2</v>
       </c>
       <c r="N23">
-        <v>0.0225</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="O23">
-        <v>0.024</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="P23">
-        <v>0.024</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="Q23">
-        <v>0.02506</v>
+        <v>3.458E-2</v>
       </c>
       <c r="R23">
-        <v>0.0226982482432751</v>
+        <v>3.5522117307272318E-2</v>
       </c>
       <c r="S23">
-        <v>0.01840847695390894</v>
+        <v>2.880874641939422E-2</v>
       </c>
       <c r="T23">
-        <v>0.02216316109494632</v>
+        <v>4.9961024163184077E-2</v>
       </c>
       <c r="U23">
-        <v>0.01574844352298058</v>
+        <v>4.4398154338798353E-2</v>
       </c>
       <c r="V23">
-        <v>0.01546498195174563</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22">
+        <v>5.3297395426919962E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.04499999999999999</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="C24">
-        <v>0.04499999999999999</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="D24">
-        <v>0.1275</v>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="E24">
-        <v>0.0975</v>
+        <v>1.35E-2</v>
       </c>
       <c r="F24">
-        <v>0.08250000000000002</v>
+        <v>1.2E-2</v>
       </c>
       <c r="G24">
-        <v>0.05399999999999999</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="H24">
-        <v>0.04499999999999999</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="I24">
-        <v>0.045</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="J24">
-        <v>0.07875</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K24">
-        <v>0.0525</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="L24">
-        <v>0.04125</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="M24">
-        <v>0.04125000000000001</v>
+        <v>7.5000000000000067E-3</v>
       </c>
       <c r="N24">
-        <v>0.036</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="O24">
-        <v>0.033</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="P24">
-        <v>0.033</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="Q24">
-        <v>0.03458</v>
+        <v>7.8399999999999997E-3</v>
       </c>
       <c r="R24">
-        <v>0.03552211730727232</v>
+        <v>7.0531279851984751E-3</v>
       </c>
       <c r="S24">
-        <v>0.02880874641939422</v>
+        <v>5.7201482060169036E-3</v>
       </c>
       <c r="T24">
-        <v>0.04996102416318408</v>
+        <v>6.8868579673562009E-3</v>
       </c>
       <c r="U24">
-        <v>0.04439815433879835</v>
+        <v>4.8935841455589359E-3</v>
       </c>
       <c r="V24">
-        <v>0.05329739542691996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22">
-      <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>0.009000000000000001</v>
-      </c>
-      <c r="C25">
-        <v>0.009000000000000001</v>
-      </c>
-      <c r="D25">
-        <v>0.01875</v>
-      </c>
-      <c r="E25">
-        <v>0.0135</v>
-      </c>
-      <c r="F25">
-        <v>0.012</v>
-      </c>
-      <c r="G25">
-        <v>0.009000000000000001</v>
-      </c>
-      <c r="H25">
-        <v>0.009000000000000001</v>
-      </c>
-      <c r="I25">
-        <v>0.0075</v>
-      </c>
-      <c r="J25">
-        <v>0.015</v>
-      </c>
-      <c r="K25">
-        <v>0.009000000000000001</v>
-      </c>
-      <c r="L25">
-        <v>0.0075</v>
-      </c>
-      <c r="M25">
-        <v>0.007500000000000007</v>
-      </c>
-      <c r="N25">
-        <v>0.0075</v>
-      </c>
-      <c r="O25">
-        <v>0.0075</v>
-      </c>
-      <c r="P25">
-        <v>0.0075</v>
-      </c>
-      <c r="Q25">
-        <v>0.00784</v>
-      </c>
-      <c r="R25">
-        <v>0.007053127985198475</v>
-      </c>
-      <c r="S25">
-        <v>0.005720148206016904</v>
-      </c>
-      <c r="T25">
-        <v>0.006886857967356201</v>
-      </c>
-      <c r="U25">
-        <v>0.004893584145558936</v>
-      </c>
-      <c r="V25">
-        <v>0.004805502866361636</v>
+        <v>4.8055028663616358E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back to the version w/o Indonesia
</commit_message>
<xml_diff>
--- a/Data/country_data/country_risk_premium.xlsx
+++ b/Data/country_data/country_risk_premium.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canne\Documents\MFE Winter\230O\prem\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A001179-A0D6-48AE-8A86-44512808EBA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2532" yWindow="1176" windowWidth="20508" windowHeight="11184" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -94,8 +88,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,14 +152,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -212,7 +198,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,27 +230,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,24 +264,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -489,16 +439,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22">
       <c r="B1" s="1">
         <v>2000</v>
       </c>
@@ -563,42 +511,42 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="C2">
         <v>0.09</v>
       </c>
       <c r="D2">
-        <v>0.13500000000000001</v>
+        <v>0.135</v>
       </c>
       <c r="E2">
-        <v>9.7500000000000003E-2</v>
+        <v>0.0975</v>
       </c>
       <c r="F2">
-        <v>9.7500000000000003E-2</v>
+        <v>0.0975</v>
       </c>
       <c r="G2">
-        <v>9.0000000000000011E-2</v>
+        <v>0.09000000000000001</v>
       </c>
       <c r="H2">
-        <v>6.7500000000000004E-2</v>
+        <v>0.0675</v>
       </c>
       <c r="I2">
-        <v>6.7500000000000004E-2</v>
+        <v>0.0675</v>
       </c>
       <c r="J2">
-        <v>0.13500000000000001</v>
+        <v>0.135</v>
       </c>
       <c r="K2">
-        <v>9.7500000000000017E-2</v>
+        <v>0.09750000000000002</v>
       </c>
       <c r="L2">
-        <v>9.0000000000000011E-2</v>
+        <v>0.09000000000000001</v>
       </c>
       <c r="M2">
         <v>0.09</v>
@@ -607,7 +555,7 @@
         <v>0.09</v>
       </c>
       <c r="O2">
-        <v>9.7500000000000003E-2</v>
+        <v>0.0975</v>
       </c>
       <c r="P2">
         <v>0.1125</v>
@@ -616,51 +564,51 @@
         <v>0.10206</v>
       </c>
       <c r="R2">
-        <v>9.2460095951420018E-2</v>
+        <v>0.09246009595142002</v>
       </c>
       <c r="S2">
-        <v>6.3441643739460193E-2</v>
+        <v>0.06344164373946019</v>
       </c>
       <c r="T2">
-        <v>7.6381515637950578E-2</v>
+        <v>0.07638151563795058</v>
       </c>
       <c r="U2">
-        <v>8.8796308677596705E-2</v>
+        <v>0.08879630867759671</v>
       </c>
       <c r="V2">
         <v>0.1162057965865632</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.4999999999999991E-2</v>
+        <v>0.04499999999999999</v>
       </c>
       <c r="C3">
-        <v>4.4999999999999991E-2</v>
+        <v>0.04499999999999999</v>
       </c>
       <c r="D3">
         <v>0.1125</v>
       </c>
       <c r="E3">
-        <v>8.2500000000000018E-2</v>
+        <v>0.08250000000000002</v>
       </c>
       <c r="F3">
         <v>0.06</v>
       </c>
       <c r="G3">
-        <v>5.3999999999999992E-2</v>
+        <v>0.05399999999999999</v>
       </c>
       <c r="H3">
-        <v>3.7500000000000012E-2</v>
+        <v>0.03750000000000001</v>
       </c>
       <c r="I3">
         <v>0.03</v>
       </c>
       <c r="J3">
-        <v>4.4999999999999998E-2</v>
+        <v>0.045</v>
       </c>
       <c r="K3">
         <v>0.03</v>
@@ -669,202 +617,202 @@
         <v>0.03</v>
       </c>
       <c r="M3">
-        <v>2.6249999999999999E-2</v>
+        <v>0.02625</v>
       </c>
       <c r="N3">
-        <v>2.6249999999999999E-2</v>
+        <v>0.02625</v>
       </c>
       <c r="O3">
-        <v>2.8500000000000001E-2</v>
+        <v>0.0285</v>
       </c>
       <c r="P3">
-        <v>2.8500000000000001E-2</v>
+        <v>0.0285</v>
       </c>
       <c r="Q3">
-        <v>4.718E-2</v>
+        <v>0.04718</v>
       </c>
       <c r="R3">
-        <v>4.2703483983110767E-2</v>
+        <v>0.04270348398311077</v>
       </c>
       <c r="S3">
-        <v>3.4632897320065983E-2</v>
+        <v>0.03463289732006598</v>
       </c>
       <c r="T3">
-        <v>4.1696794602356632E-2</v>
+        <v>0.04169679460235663</v>
       </c>
       <c r="U3">
-        <v>2.962842764492955E-2</v>
+        <v>0.02962842764492955</v>
       </c>
       <c r="V3">
-        <v>2.9095135536334991E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.02909513553633499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="C4">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="D4">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="E4">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="F4">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="G4">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="H4">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="I4">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="J4">
-        <v>2.1000000000000001E-2</v>
+        <v>0.021</v>
       </c>
       <c r="K4">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="L4">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="M4">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="N4">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="O4">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="P4">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="Q4">
-        <v>9.5199999999999989E-3</v>
+        <v>0.009519999999999999</v>
       </c>
       <c r="R4">
-        <v>8.5919922728781434E-3</v>
+        <v>0.008591992272878143</v>
       </c>
       <c r="S4">
-        <v>6.9681805418751368E-3</v>
+        <v>0.006968180541875137</v>
       </c>
       <c r="T4">
-        <v>9.7668167537051567E-3</v>
+        <v>0.009766816753705157</v>
       </c>
       <c r="U4">
-        <v>6.9399920609744909E-3</v>
+        <v>0.006939992060974491</v>
       </c>
       <c r="V4">
-        <v>6.8150767922946836E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.006815076792294684</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>9.5000000000000015E-3</v>
+        <v>0.009500000000000001</v>
       </c>
       <c r="C5">
-        <v>9.5000000000000015E-3</v>
+        <v>0.009500000000000001</v>
       </c>
       <c r="D5">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="E5">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="F5">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="G5">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="H5">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="I5">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="J5">
-        <v>2.1000000000000001E-2</v>
+        <v>0.021</v>
       </c>
       <c r="K5">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="L5">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="M5">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="N5">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="O5">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="P5">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="Q5">
-        <v>9.5199999999999989E-3</v>
+        <v>0.009519999999999999</v>
       </c>
       <c r="R5">
-        <v>8.5919922728781434E-3</v>
+        <v>0.008591992272878143</v>
       </c>
       <c r="S5">
-        <v>8.1122101830785175E-3</v>
+        <v>0.008112210183078518</v>
       </c>
       <c r="T5">
-        <v>9.7668167537051567E-3</v>
+        <v>0.009766816753705157</v>
       </c>
       <c r="U5">
-        <v>6.9399920609744909E-3</v>
+        <v>0.006939992060974491</v>
       </c>
       <c r="V5">
-        <v>6.8150767922946836E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.006815076792294684</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.0000000000000009E-2</v>
+        <v>0.03000000000000001</v>
       </c>
       <c r="C6">
-        <v>3.0000000000000009E-2</v>
+        <v>0.03000000000000001</v>
       </c>
       <c r="D6">
-        <v>2.6249999999999999E-2</v>
+        <v>0.02625</v>
       </c>
       <c r="E6">
-        <v>1.95E-2</v>
+        <v>0.0195</v>
       </c>
       <c r="F6">
-        <v>1.95E-2</v>
+        <v>0.0195</v>
       </c>
       <c r="G6">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="H6">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="I6">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="J6">
-        <v>3.8999999999999993E-2</v>
+        <v>0.03899999999999999</v>
       </c>
       <c r="K6">
         <v>0.03</v>
@@ -879,72 +827,72 @@
         <v>0.03</v>
       </c>
       <c r="O6">
-        <v>3.3000000000000002E-2</v>
+        <v>0.033</v>
       </c>
       <c r="P6">
-        <v>2.8500000000000001E-2</v>
+        <v>0.0285</v>
       </c>
       <c r="Q6">
-        <v>2.9819999999999999E-2</v>
+        <v>0.02982</v>
       </c>
       <c r="R6">
-        <v>2.7058363725034149E-2</v>
+        <v>0.02705836372503415</v>
       </c>
       <c r="S6">
-        <v>2.1944568572173941E-2</v>
+        <v>0.02194456857217394</v>
       </c>
       <c r="T6">
-        <v>2.6420491474766512E-2</v>
+        <v>0.02642049147476651</v>
       </c>
       <c r="U6">
-        <v>1.8773568267507919E-2</v>
+        <v>0.01877356826750792</v>
       </c>
       <c r="V6">
-        <v>1.8435656450951E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.018435656450951</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="C7">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="D7">
-        <v>2.2499999999999989E-2</v>
+        <v>0.02249999999999999</v>
       </c>
       <c r="E7">
-        <v>1.8000000000000009E-2</v>
+        <v>0.01800000000000001</v>
       </c>
       <c r="F7">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="G7">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="H7">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="I7">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="J7">
-        <v>4.4999999999999998E-2</v>
+        <v>0.045</v>
       </c>
       <c r="K7">
-        <v>3.7500000000000012E-2</v>
+        <v>0.03750000000000001</v>
       </c>
       <c r="L7">
-        <v>3.5999999999999997E-2</v>
+        <v>0.036</v>
       </c>
       <c r="M7">
-        <v>7.5000000000000011E-2</v>
+        <v>0.07500000000000001</v>
       </c>
       <c r="N7">
-        <v>7.5000000000000011E-2</v>
+        <v>0.07500000000000001</v>
       </c>
       <c r="O7">
         <v>0.1125</v>
@@ -956,57 +904,57 @@
         <v>0.10206</v>
       </c>
       <c r="R7">
-        <v>9.2460095951420018E-2</v>
+        <v>0.09246009595142002</v>
       </c>
       <c r="S7">
-        <v>7.4985942846148873E-2</v>
+        <v>0.07498594284614887</v>
       </c>
       <c r="T7">
-        <v>9.028044717206947E-2</v>
+        <v>0.09028044717206947</v>
       </c>
       <c r="U7">
-        <v>5.4274296887108192E-2</v>
+        <v>0.05427429688710819</v>
       </c>
       <c r="V7">
-        <v>5.3297395426919962E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.05329739542691996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>9.5000000000000015E-3</v>
+        <v>0.009500000000000001</v>
       </c>
       <c r="C8">
-        <v>5.9999999999999984E-3</v>
+        <v>0.005999999999999998</v>
       </c>
       <c r="D8">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="E8">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="F8">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="G8">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="H8">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="I8">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="J8">
-        <v>2.1000000000000001E-2</v>
+        <v>0.021</v>
       </c>
       <c r="K8">
-        <v>1.575E-2</v>
+        <v>0.01575</v>
       </c>
       <c r="L8">
-        <v>3.5999999999999997E-2</v>
+        <v>0.036</v>
       </c>
       <c r="M8">
         <v>0.105</v>
@@ -1030,51 +978,51 @@
         <v>0.1037946892655431</v>
       </c>
       <c r="T8">
-        <v>9.028044717206947E-2</v>
+        <v>0.09028044717206947</v>
       </c>
       <c r="U8">
-        <v>4.4398154338798353E-2</v>
+        <v>0.04439815433879835</v>
       </c>
       <c r="V8">
-        <v>3.4861738975968962E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.03486173897596896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>3.0000000000000009E-2</v>
+        <v>0.03000000000000001</v>
       </c>
       <c r="C9">
-        <v>3.0000000000000009E-2</v>
+        <v>0.03000000000000001</v>
       </c>
       <c r="D9">
         <v>0.06</v>
       </c>
       <c r="E9">
-        <v>2.1749999999999999E-2</v>
+        <v>0.02175</v>
       </c>
       <c r="F9">
-        <v>4.4999999999999998E-2</v>
+        <v>0.045</v>
       </c>
       <c r="G9">
-        <v>4.0499999999999987E-2</v>
+        <v>0.04049999999999999</v>
       </c>
       <c r="H9">
-        <v>3.7500000000000012E-2</v>
+        <v>0.03750000000000001</v>
       </c>
       <c r="I9">
-        <v>3.7500000000000012E-2</v>
+        <v>0.03750000000000001</v>
       </c>
       <c r="J9">
         <v>0.06</v>
       </c>
       <c r="K9">
-        <v>4.4999999999999998E-2</v>
+        <v>0.045</v>
       </c>
       <c r="L9">
-        <v>3.5999999999999997E-2</v>
+        <v>0.036</v>
       </c>
       <c r="M9">
         <v>0.03</v>
@@ -1083,270 +1031,270 @@
         <v>0.03</v>
       </c>
       <c r="O9">
-        <v>3.3000000000000002E-2</v>
+        <v>0.033</v>
       </c>
       <c r="P9">
-        <v>3.3000000000000002E-2</v>
+        <v>0.033</v>
       </c>
       <c r="Q9">
-        <v>3.458E-2</v>
+        <v>0.03458</v>
       </c>
       <c r="R9">
-        <v>3.1290240516153242E-2</v>
+        <v>0.03129024051615324</v>
       </c>
       <c r="S9">
-        <v>2.1944568572173941E-2</v>
+        <v>0.02194456857217394</v>
       </c>
       <c r="T9">
-        <v>2.6420491474766512E-2</v>
+        <v>0.02642049147476651</v>
       </c>
       <c r="U9">
-        <v>1.8773568267507919E-2</v>
+        <v>0.01877356826750792</v>
       </c>
       <c r="V9">
-        <v>2.1318958170767989E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.02131895817076799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.2999999999999999E-2</v>
+        <v>0.013</v>
       </c>
       <c r="C10">
-        <v>1.2999999999999999E-2</v>
+        <v>0.013</v>
       </c>
       <c r="D10">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="E10">
-        <v>1.4250000000000001E-2</v>
+        <v>0.01425</v>
       </c>
       <c r="F10">
-        <v>1.4250000000000001E-2</v>
+        <v>0.01425</v>
       </c>
       <c r="G10">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="H10">
-        <v>1.2749999999999999E-2</v>
+        <v>0.01275</v>
       </c>
       <c r="I10">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="J10">
-        <v>2.4000000000000011E-2</v>
+        <v>0.02400000000000001</v>
       </c>
       <c r="K10">
-        <v>1.575E-2</v>
+        <v>0.01575</v>
       </c>
       <c r="L10">
-        <v>1.2749999999999999E-2</v>
+        <v>0.01275</v>
       </c>
       <c r="M10">
-        <v>1.2749999999999999E-2</v>
+        <v>0.01275</v>
       </c>
       <c r="N10">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="O10">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="P10">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="Q10">
-        <v>7.8399999999999997E-3</v>
+        <v>0.00784</v>
       </c>
       <c r="R10">
-        <v>7.0531279851984751E-3</v>
+        <v>0.007053127985198475</v>
       </c>
       <c r="S10">
-        <v>5.7201482060169036E-3</v>
+        <v>0.005720148206016904</v>
       </c>
       <c r="T10">
-        <v>6.8868579673562009E-3</v>
+        <v>0.006886857967356201</v>
       </c>
       <c r="U10">
-        <v>4.8935841455589359E-3</v>
+        <v>0.004893584145558936</v>
       </c>
       <c r="V10">
-        <v>4.8055028663616358E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.004805502866361636</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.2999999999999999E-2</v>
+        <v>0.013</v>
       </c>
       <c r="C11">
-        <v>1.2999999999999999E-2</v>
+        <v>0.013</v>
       </c>
       <c r="D11">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="E11">
-        <v>1.4250000000000001E-2</v>
+        <v>0.01425</v>
       </c>
       <c r="F11">
-        <v>1.4250000000000001E-2</v>
+        <v>0.01425</v>
       </c>
       <c r="G11">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="H11">
-        <v>1.2749999999999999E-2</v>
+        <v>0.01275</v>
       </c>
       <c r="I11">
-        <v>1.2749999999999999E-2</v>
+        <v>0.01275</v>
       </c>
       <c r="J11">
-        <v>2.6250000000000009E-2</v>
+        <v>0.02625000000000001</v>
       </c>
       <c r="K11">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="L11">
-        <v>1.7250000000000001E-2</v>
+        <v>0.01725</v>
       </c>
       <c r="M11">
-        <v>1.7250000000000001E-2</v>
+        <v>0.01725</v>
       </c>
       <c r="N11">
-        <v>1.7250000000000001E-2</v>
+        <v>0.01725</v>
       </c>
       <c r="O11">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="P11">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="Q11">
-        <v>1.89E-2</v>
+        <v>0.0189</v>
       </c>
       <c r="R11">
-        <v>1.7055745855116319E-2</v>
+        <v>0.01705574585511632</v>
       </c>
       <c r="S11">
-        <v>1.383235838909542E-2</v>
+        <v>0.01383235838909542</v>
       </c>
       <c r="T11">
-        <v>1.665367472106136E-2</v>
+        <v>0.01665367472106136</v>
       </c>
       <c r="U11">
-        <v>1.1833576206533429E-2</v>
+        <v>0.01183357620653343</v>
       </c>
       <c r="V11">
-        <v>1.1620579658656319E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.01162057965865632</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1.4500000000000009E-2</v>
+        <v>0.01450000000000001</v>
       </c>
       <c r="C12">
-        <v>1.4500000000000009E-2</v>
+        <v>0.01450000000000001</v>
       </c>
       <c r="D12">
-        <v>2.2499999999999989E-2</v>
+        <v>0.02249999999999999</v>
       </c>
       <c r="E12">
-        <v>1.8000000000000009E-2</v>
+        <v>0.01800000000000001</v>
       </c>
       <c r="F12">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="G12">
-        <v>1.6500000000000001E-2</v>
+        <v>0.0165</v>
       </c>
       <c r="H12">
-        <v>1.4999999999999991E-2</v>
+        <v>0.01499999999999999</v>
       </c>
       <c r="I12">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="J12">
         <v>0.03</v>
       </c>
       <c r="K12">
-        <v>2.4000000000000011E-2</v>
+        <v>0.02400000000000001</v>
       </c>
       <c r="L12">
-        <v>2.250000000000001E-2</v>
+        <v>0.02250000000000001</v>
       </c>
       <c r="M12">
-        <v>2.2499999999999989E-2</v>
+        <v>0.02249999999999999</v>
       </c>
       <c r="N12">
-        <v>2.2499999999999999E-2</v>
+        <v>0.0225</v>
       </c>
       <c r="O12">
-        <v>2.4E-2</v>
+        <v>0.024</v>
       </c>
       <c r="P12">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="Q12">
-        <v>1.89E-2</v>
+        <v>0.0189</v>
       </c>
       <c r="R12">
-        <v>1.7055745855116319E-2</v>
+        <v>0.01705574585511632</v>
       </c>
       <c r="S12">
-        <v>1.383235838909542E-2</v>
+        <v>0.01383235838909542</v>
       </c>
       <c r="T12">
-        <v>1.665367472106136E-2</v>
+        <v>0.01665367472106136</v>
       </c>
       <c r="U12">
-        <v>1.1833576206533429E-2</v>
+        <v>0.01183357620653343</v>
       </c>
       <c r="V12">
-        <v>1.5464981951745629E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.01546498195174563</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>7.4999999999999983E-2</v>
+        <v>0.07499999999999998</v>
       </c>
       <c r="C13">
-        <v>7.4999999999999983E-2</v>
+        <v>0.07499999999999998</v>
       </c>
       <c r="D13">
         <v>0.1275</v>
       </c>
       <c r="E13">
-        <v>8.2500000000000018E-2</v>
+        <v>0.08250000000000002</v>
       </c>
       <c r="F13">
-        <v>8.2500000000000018E-2</v>
+        <v>0.08250000000000002</v>
       </c>
       <c r="G13">
-        <v>7.5000000000000011E-2</v>
+        <v>0.07500000000000001</v>
       </c>
       <c r="H13">
-        <v>5.2499999999999998E-2</v>
+        <v>0.0525</v>
       </c>
       <c r="I13">
-        <v>5.2499999999999998E-2</v>
+        <v>0.0525</v>
       </c>
       <c r="J13">
-        <v>0.13500000000000001</v>
+        <v>0.135</v>
       </c>
       <c r="K13">
-        <v>9.7500000000000017E-2</v>
+        <v>0.09750000000000002</v>
       </c>
       <c r="L13">
-        <v>9.0000000000000011E-2</v>
+        <v>0.09000000000000001</v>
       </c>
       <c r="M13">
         <v>0.09</v>
@@ -1364,22 +1312,22 @@
         <v>0.10206</v>
       </c>
       <c r="R13">
-        <v>9.2460095951420018E-2</v>
+        <v>0.09246009595142002</v>
       </c>
       <c r="S13">
-        <v>7.4985942846148873E-2</v>
+        <v>0.07498594284614887</v>
       </c>
       <c r="T13">
-        <v>9.028044717206947E-2</v>
+        <v>0.09028044717206947</v>
       </c>
       <c r="U13">
-        <v>6.4150439435418039E-2</v>
+        <v>0.06415043943541804</v>
       </c>
       <c r="V13">
-        <v>6.2995773939031607E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.06299577393903161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1393,22 +1341,22 @@
         <v>0.03</v>
       </c>
       <c r="E14">
-        <v>2.1749999999999999E-2</v>
+        <v>0.02175</v>
       </c>
       <c r="F14">
-        <v>2.1750000000000009E-2</v>
+        <v>0.02175000000000001</v>
       </c>
       <c r="G14">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="H14">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="I14">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="J14">
-        <v>3.8999999999999993E-2</v>
+        <v>0.03899999999999999</v>
       </c>
       <c r="K14">
         <v>0.03</v>
@@ -1420,243 +1368,243 @@
         <v>0.03</v>
       </c>
       <c r="N14">
-        <v>2.6249999999999999E-2</v>
+        <v>0.02625</v>
       </c>
       <c r="O14">
-        <v>2.8500000000000001E-2</v>
+        <v>0.0285</v>
       </c>
       <c r="P14">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="Q14">
-        <v>1.89E-2</v>
+        <v>0.0189</v>
       </c>
       <c r="R14">
-        <v>1.7055745855116319E-2</v>
+        <v>0.01705574585511632</v>
       </c>
       <c r="S14">
-        <v>1.383235838909542E-2</v>
+        <v>0.01383235838909542</v>
       </c>
       <c r="T14">
-        <v>1.665367472106136E-2</v>
+        <v>0.01665367472106136</v>
       </c>
       <c r="U14">
-        <v>1.1833576206533429E-2</v>
+        <v>0.01183357620653343</v>
       </c>
       <c r="V14">
-        <v>1.1620579658656319E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.01162057965865632</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="C15">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="D15">
         <v>0.03</v>
       </c>
       <c r="E15">
-        <v>2.1749999999999999E-2</v>
+        <v>0.02175</v>
       </c>
       <c r="F15">
-        <v>4.4999999999999998E-2</v>
+        <v>0.045</v>
       </c>
       <c r="G15">
         <v>0.06</v>
       </c>
       <c r="H15">
-        <v>5.2499999999999998E-2</v>
+        <v>0.0525</v>
       </c>
       <c r="I15">
-        <v>5.2499999999999998E-2</v>
+        <v>0.0525</v>
       </c>
       <c r="J15">
-        <v>9.7500000000000017E-2</v>
+        <v>0.09750000000000002</v>
       </c>
       <c r="K15">
-        <v>5.2499999999999998E-2</v>
+        <v>0.0525</v>
       </c>
       <c r="L15">
-        <v>4.8750000000000002E-2</v>
+        <v>0.04875</v>
       </c>
       <c r="M15">
-        <v>4.1250000000000009E-2</v>
+        <v>0.04125000000000001</v>
       </c>
       <c r="N15">
-        <v>3.5999999999999997E-2</v>
+        <v>0.036</v>
       </c>
       <c r="O15">
-        <v>3.3000000000000002E-2</v>
+        <v>0.033</v>
       </c>
       <c r="P15">
-        <v>2.8500000000000001E-2</v>
+        <v>0.0285</v>
       </c>
       <c r="Q15">
-        <v>2.9819999999999999E-2</v>
+        <v>0.02982</v>
       </c>
       <c r="R15">
-        <v>2.7058363725034149E-2</v>
+        <v>0.02705836372503415</v>
       </c>
       <c r="S15">
-        <v>2.1944568572173941E-2</v>
+        <v>0.02194456857217394</v>
       </c>
       <c r="T15">
-        <v>2.6420491474766512E-2</v>
+        <v>0.02642049147476651</v>
       </c>
       <c r="U15">
-        <v>1.8773568267507919E-2</v>
+        <v>0.01877356826750792</v>
       </c>
       <c r="V15">
-        <v>1.8435656450951E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.018435656450951</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="C16">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="D16">
-        <v>1.8749999999999999E-2</v>
+        <v>0.01875</v>
       </c>
       <c r="E16">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="F16">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="G16">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="H16">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="I16">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="J16">
-        <v>2.4000000000000011E-2</v>
+        <v>0.02400000000000001</v>
       </c>
       <c r="K16">
-        <v>1.575E-2</v>
+        <v>0.01575</v>
       </c>
       <c r="L16">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="M16">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="N16">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="O16">
-        <v>1.2749999999999999E-2</v>
+        <v>0.01275</v>
       </c>
       <c r="P16">
-        <v>1.2749999999999999E-2</v>
+        <v>0.01275</v>
       </c>
       <c r="Q16">
-        <v>1.3299999999999999E-2</v>
+        <v>0.0133</v>
       </c>
       <c r="R16">
-        <v>1.20544369201574E-2</v>
+        <v>0.0120544369201574</v>
       </c>
       <c r="S16">
-        <v>9.7762532975561641E-3</v>
+        <v>0.009776253297556164</v>
       </c>
       <c r="T16">
-        <v>1.1770266344208779E-2</v>
+        <v>0.01177026634420878</v>
       </c>
       <c r="U16">
-        <v>8.36358017604618E-3</v>
+        <v>0.00836358017604618</v>
       </c>
       <c r="V16">
-        <v>8.2130412625089771E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.008213041262508977</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>1.2999999999999999E-2</v>
+        <v>0.013</v>
       </c>
       <c r="C17">
-        <v>1.2999999999999999E-2</v>
+        <v>0.013</v>
       </c>
       <c r="D17">
-        <v>2.0250000000000001E-2</v>
+        <v>0.02025</v>
       </c>
       <c r="E17">
-        <v>1.4250000000000001E-2</v>
+        <v>0.01425</v>
       </c>
       <c r="F17">
-        <v>1.4250000000000001E-2</v>
+        <v>0.01425</v>
       </c>
       <c r="G17">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="H17">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="I17">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="J17">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="K17">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="L17">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="M17">
-        <v>7.5000000000000067E-3</v>
+        <v>0.007500000000000007</v>
       </c>
       <c r="N17">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="O17">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="P17">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="Q17">
-        <v>7.8399999999999997E-3</v>
+        <v>0.00784</v>
       </c>
       <c r="R17">
-        <v>7.0531279851984751E-3</v>
+        <v>0.007053127985198475</v>
       </c>
       <c r="S17">
-        <v>6.9681805418751368E-3</v>
+        <v>0.006968180541875137</v>
       </c>
       <c r="T17">
-        <v>8.389445160233917E-3</v>
+        <v>0.008389445160233917</v>
       </c>
       <c r="U17">
-        <v>5.9612752318627038E-3</v>
+        <v>0.005961275231862704</v>
       </c>
       <c r="V17">
-        <v>5.8539762190223561E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.005853976219022356</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="C18">
         <v>0.04</v>
@@ -1665,466 +1613,466 @@
         <v>0.06</v>
       </c>
       <c r="E18">
-        <v>2.1749999999999999E-2</v>
+        <v>0.02175</v>
       </c>
       <c r="F18">
-        <v>2.1750000000000009E-2</v>
+        <v>0.02175000000000001</v>
       </c>
       <c r="G18">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="H18">
-        <v>1.7249999999999991E-2</v>
+        <v>0.01724999999999999</v>
       </c>
       <c r="I18">
-        <v>1.7250000000000001E-2</v>
+        <v>0.01725</v>
       </c>
       <c r="J18">
         <v>0.03</v>
       </c>
       <c r="K18">
-        <v>2.4000000000000011E-2</v>
+        <v>0.02400000000000001</v>
       </c>
       <c r="L18">
-        <v>2.250000000000001E-2</v>
+        <v>0.02250000000000001</v>
       </c>
       <c r="M18">
-        <v>2.2499999999999989E-2</v>
+        <v>0.02249999999999999</v>
       </c>
       <c r="N18">
-        <v>2.2499999999999999E-2</v>
+        <v>0.0225</v>
       </c>
       <c r="O18">
-        <v>2.4E-2</v>
+        <v>0.024</v>
       </c>
       <c r="P18">
-        <v>2.8500000000000001E-2</v>
+        <v>0.0285</v>
       </c>
       <c r="Q18">
-        <v>3.9199999999999999E-2</v>
+        <v>0.0392</v>
       </c>
       <c r="R18">
-        <v>3.5522117307272318E-2</v>
+        <v>0.03552211730727232</v>
       </c>
       <c r="S18">
-        <v>2.880874641939422E-2</v>
+        <v>0.02880874641939422</v>
       </c>
       <c r="T18">
-        <v>3.468472103559396E-2</v>
+        <v>0.03468472103559396</v>
       </c>
       <c r="U18">
-        <v>2.1709718754843281E-2</v>
+        <v>0.02170971875484328</v>
       </c>
       <c r="V18">
-        <v>2.1318958170767989E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.02131895817076799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1.4500000000000009E-2</v>
+        <v>0.01450000000000001</v>
       </c>
       <c r="C19">
-        <v>1.4500000000000009E-2</v>
+        <v>0.01450000000000001</v>
       </c>
       <c r="D19">
-        <v>4.8750000000000002E-2</v>
+        <v>0.04875</v>
       </c>
       <c r="E19">
-        <v>1.8000000000000009E-2</v>
+        <v>0.01800000000000001</v>
       </c>
       <c r="F19">
-        <v>1.95E-2</v>
+        <v>0.0195</v>
       </c>
       <c r="G19">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="H19">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="I19">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="J19">
-        <v>2.1000000000000001E-2</v>
+        <v>0.021</v>
       </c>
       <c r="K19">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="L19">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="M19">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="N19">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="O19">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="P19">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="Q19">
-        <v>1.106E-2</v>
+        <v>0.01106</v>
       </c>
       <c r="R19">
-        <v>1.0002617869917839E-2</v>
+        <v>0.01000261786991784</v>
       </c>
       <c r="S19">
-        <v>8.1122101830785175E-3</v>
+        <v>0.008112210183078518</v>
       </c>
       <c r="T19">
-        <v>9.7668167537051567E-3</v>
+        <v>0.009766816753705157</v>
       </c>
       <c r="U19">
-        <v>6.9399920609744909E-3</v>
+        <v>0.006939992060974491</v>
       </c>
       <c r="V19">
-        <v>6.8150767922946836E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.006815076792294684</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1.4500000000000009E-2</v>
+        <v>0.01450000000000001</v>
       </c>
       <c r="C20">
-        <v>1.2999999999999999E-2</v>
+        <v>0.013</v>
       </c>
       <c r="D20">
-        <v>1.8749999999999999E-2</v>
+        <v>0.01875</v>
       </c>
       <c r="E20">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="F20">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="G20">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="H20">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="I20">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="J20">
-        <v>2.4000000000000011E-2</v>
+        <v>0.02400000000000001</v>
       </c>
       <c r="K20">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="L20">
-        <v>1.7250000000000001E-2</v>
+        <v>0.01725</v>
       </c>
       <c r="M20">
-        <v>1.7250000000000001E-2</v>
+        <v>0.01725</v>
       </c>
       <c r="N20">
-        <v>2.2499999999999999E-2</v>
+        <v>0.0225</v>
       </c>
       <c r="O20">
-        <v>2.4E-2</v>
+        <v>0.024</v>
       </c>
       <c r="P20">
-        <v>2.8500000000000001E-2</v>
+        <v>0.0285</v>
       </c>
       <c r="Q20">
-        <v>2.9819999999999999E-2</v>
+        <v>0.02982</v>
       </c>
       <c r="R20">
-        <v>2.7058363725034149E-2</v>
+        <v>0.02705836372503415</v>
       </c>
       <c r="S20">
-        <v>2.5376657495784081E-2</v>
+        <v>0.02537665749578408</v>
       </c>
       <c r="T20">
-        <v>3.0552606255180231E-2</v>
+        <v>0.03055260625518023</v>
       </c>
       <c r="U20">
-        <v>2.1709718754843281E-2</v>
+        <v>0.02170971875484328</v>
       </c>
       <c r="V20">
-        <v>2.9095135536334991E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.02909513553633499</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="C21">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="D21">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="E21">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="F21">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="I21">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="J21">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="K21">
-        <v>1.125E-2</v>
+        <v>0.01125</v>
       </c>
       <c r="L21">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="M21">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="N21">
-        <v>1.0500000000000001E-2</v>
+        <v>0.0105</v>
       </c>
       <c r="O21">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="P21">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="Q21">
-        <v>9.5199999999999989E-3</v>
+        <v>0.009519999999999999</v>
       </c>
       <c r="R21">
-        <v>8.5919922728781434E-3</v>
+        <v>0.008591992272878143</v>
       </c>
       <c r="S21">
-        <v>6.9681805418751368E-3</v>
+        <v>0.006968180541875137</v>
       </c>
       <c r="T21">
-        <v>8.389445160233917E-3</v>
+        <v>0.008389445160233917</v>
       </c>
       <c r="U21">
-        <v>5.9612752318627038E-3</v>
+        <v>0.005961275231862704</v>
       </c>
       <c r="V21">
-        <v>5.8539762190223561E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.005853976219022356</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1.4500000000000009E-2</v>
+        <v>0.01450000000000001</v>
       </c>
       <c r="C22">
-        <v>1.4500000000000009E-2</v>
+        <v>0.01450000000000001</v>
       </c>
       <c r="D22">
-        <v>2.2499999999999989E-2</v>
+        <v>0.02249999999999999</v>
       </c>
       <c r="E22">
-        <v>1.8000000000000009E-2</v>
+        <v>0.01800000000000001</v>
       </c>
       <c r="F22">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="G22">
-        <v>1.6500000000000001E-2</v>
+        <v>0.0165</v>
       </c>
       <c r="H22">
-        <v>1.4999999999999991E-2</v>
+        <v>0.01499999999999999</v>
       </c>
       <c r="I22">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="J22">
         <v>0.03</v>
       </c>
       <c r="K22">
-        <v>2.4000000000000011E-2</v>
+        <v>0.02400000000000001</v>
       </c>
       <c r="L22">
-        <v>2.250000000000001E-2</v>
+        <v>0.02250000000000001</v>
       </c>
       <c r="M22">
-        <v>2.2499999999999989E-2</v>
+        <v>0.02249999999999999</v>
       </c>
       <c r="N22">
-        <v>2.2499999999999999E-2</v>
+        <v>0.0225</v>
       </c>
       <c r="O22">
-        <v>2.4E-2</v>
+        <v>0.024</v>
       </c>
       <c r="P22">
-        <v>2.4E-2</v>
+        <v>0.024</v>
       </c>
       <c r="Q22">
-        <v>2.5059999999999999E-2</v>
+        <v>0.02506</v>
       </c>
       <c r="R22">
-        <v>2.2698248243275099E-2</v>
+        <v>0.0226982482432751</v>
       </c>
       <c r="S22">
-        <v>1.8408476953908941E-2</v>
+        <v>0.01840847695390894</v>
       </c>
       <c r="T22">
-        <v>2.2163161094946319E-2</v>
+        <v>0.02216316109494632</v>
       </c>
       <c r="U22">
-        <v>1.574844352298058E-2</v>
+        <v>0.01574844352298058</v>
       </c>
       <c r="V22">
-        <v>1.5464981951745629E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.01546498195174563</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>4.4999999999999991E-2</v>
+        <v>0.04499999999999999</v>
       </c>
       <c r="C23">
-        <v>4.4999999999999991E-2</v>
+        <v>0.04499999999999999</v>
       </c>
       <c r="D23">
         <v>0.1275</v>
       </c>
       <c r="E23">
-        <v>9.7500000000000003E-2</v>
+        <v>0.0975</v>
       </c>
       <c r="F23">
-        <v>8.2500000000000018E-2</v>
+        <v>0.08250000000000002</v>
       </c>
       <c r="G23">
-        <v>5.3999999999999992E-2</v>
+        <v>0.05399999999999999</v>
       </c>
       <c r="H23">
-        <v>4.4999999999999991E-2</v>
+        <v>0.04499999999999999</v>
       </c>
       <c r="I23">
-        <v>4.4999999999999998E-2</v>
+        <v>0.045</v>
       </c>
       <c r="J23">
-        <v>7.8750000000000001E-2</v>
+        <v>0.07875</v>
       </c>
       <c r="K23">
-        <v>5.2499999999999998E-2</v>
+        <v>0.0525</v>
       </c>
       <c r="L23">
-        <v>4.1250000000000002E-2</v>
+        <v>0.04125</v>
       </c>
       <c r="M23">
-        <v>4.1250000000000009E-2</v>
+        <v>0.04125000000000001</v>
       </c>
       <c r="N23">
-        <v>3.5999999999999997E-2</v>
+        <v>0.036</v>
       </c>
       <c r="O23">
-        <v>3.3000000000000002E-2</v>
+        <v>0.033</v>
       </c>
       <c r="P23">
-        <v>3.3000000000000002E-2</v>
+        <v>0.033</v>
       </c>
       <c r="Q23">
-        <v>3.458E-2</v>
+        <v>0.03458</v>
       </c>
       <c r="R23">
-        <v>3.5522117307272318E-2</v>
+        <v>0.03552211730727232</v>
       </c>
       <c r="S23">
-        <v>2.880874641939422E-2</v>
+        <v>0.02880874641939422</v>
       </c>
       <c r="T23">
-        <v>4.9961024163184077E-2</v>
+        <v>0.04996102416318408</v>
       </c>
       <c r="U23">
-        <v>4.4398154338798353E-2</v>
+        <v>0.04439815433879835</v>
       </c>
       <c r="V23">
-        <v>5.3297395426919962E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.05329739542691996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="C24">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="D24">
-        <v>1.8749999999999999E-2</v>
+        <v>0.01875</v>
       </c>
       <c r="E24">
-        <v>1.35E-2</v>
+        <v>0.0135</v>
       </c>
       <c r="F24">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="G24">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="H24">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="I24">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="J24">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="K24">
-        <v>9.0000000000000011E-3</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="L24">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="M24">
-        <v>7.5000000000000067E-3</v>
+        <v>0.007500000000000007</v>
       </c>
       <c r="N24">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="O24">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="P24">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="Q24">
-        <v>7.8399999999999997E-3</v>
+        <v>0.00784</v>
       </c>
       <c r="R24">
-        <v>7.0531279851984751E-3</v>
+        <v>0.007053127985198475</v>
       </c>
       <c r="S24">
-        <v>5.7201482060169036E-3</v>
+        <v>0.005720148206016904</v>
       </c>
       <c r="T24">
-        <v>6.8868579673562009E-3</v>
+        <v>0.006886857967356201</v>
       </c>
       <c r="U24">
-        <v>4.8935841455589359E-3</v>
+        <v>0.004893584145558936</v>
       </c>
       <c r="V24">
-        <v>4.8055028663616358E-3</v>
+        <v>0.004805502866361636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>